<commit_message>
backend: MERN Project 28 - Memvalidasi Request Body dan Memberikan Error Response yang Dinamis
</commit_message>
<xml_diff>
--- a/backend/mern-api/docs/api-planning.xlsx
+++ b/backend/mern-api/docs/api-planning.xlsx
@@ -72,12 +72,12 @@
     <t>{
     "name":"Testing",
     "email":"test@gmail.com",
-    "password":"123456",
+    "password":"123456"
 }</t>
   </si>
   <si>
     <t>{
-    "kode":"200",
+    "code":"200",
     "message":"Successfully registered access",
     "data":{
         "name":"Testing",
@@ -87,7 +87,7 @@
   </si>
   <si>
     <t>{
-    "kode":"400",
+    "code":"400",
     "message":"email tidak valid"
 }</t>
   </si>
@@ -100,12 +100,12 @@
   <si>
     <t>{ 
     "email":"test@gmail.com",
-    "password":"123456",
+    "password":"123456"
 }</t>
   </si>
   <si>
     <t>{
-    "kode":"200",
+    "code":"200",
     "message":"Successfully login",
     "data":{
         "id":"123",
@@ -115,7 +115,7 @@
   </si>
   <si>
     <t>{
-    "kode":"400",
+    "code":"400",
     "message":"Password salah"
 }</t>
   </si>
@@ -127,18 +127,18 @@
   </si>
   <si>
     <t>{
-    "userId":"123", 
+    "userId":"123"
 }</t>
   </si>
   <si>
     <t>{
-    "kode":"200",
-    "message":"Successfully logout",
+    "code":"200",
+    "message":"Successfully logout"
 }</t>
   </si>
   <si>
     <t>{
-    "kode":"500",
+    "code":"500",
     "message":"Internal Server Error"
 }</t>
   </si>
@@ -153,58 +153,64 @@
   </si>
   <si>
     <t>{
-  "title_post": "Harry potter book 1",
-  "author_post": "JK Rowling",
-  "date_post": "2024-08-21",
-  "body_post": "Once upon a time bla bla bla"
-  "thumb_image": file
+  "title_post": "Harry potter book 1",  
+  "body_post": "Once upon a time bla bla bla",
+  "thumb_image": image.JPG
   "user_id": 123
 }</t>
   </si>
   <si>
     <t>{
-    "kode":"200",
+    "code":"200",
     "message":"Successfully added data",
+    "data": {
+            "title_post": "Harry potter book 1",  
+            "body_post": "Once upon a time bla bla bla",
+            "thumb_image": "image.JPG",
+            "author": {
+                "user_id": 1,
+                "name": "Testing"
+            }
+    }
+}</t>
+  </si>
+  <si>
+    <t>{
+    "code":"400",
+    "message":"Judul post sudah ada"
+}</t>
+  </si>
+  <si>
+    <t>2. Get Post</t>
+  </si>
+  <si>
+    <t>GET</t>
+  </si>
+  <si>
+    <t>{
+    "code":"200",
+    "message":"Successfully updated data"
     "data": {}
 }</t>
   </si>
   <si>
+    <t>3. Update Post</t>
+  </si>
+  <si>
+    <t>PUT</t>
+  </si>
+  <si>
+    <t>{root.api}/{version}/blog/post/:post-id</t>
+  </si>
+  <si>
     <t>{
-    "kode":"400",
-    "message":"Judul post sudah ada"
+    "code":"200",
+    "message":"Successfully updated data"
 }</t>
   </si>
   <si>
-    <t>2. Get Post</t>
-  </si>
-  <si>
-    <t>GET</t>
-  </si>
-  <si>
     <t>{
-    "kode":"200",
-    "message":"Successfully updated data",
-    "data": {}
-}</t>
-  </si>
-  <si>
-    <t>3. Update Post</t>
-  </si>
-  <si>
-    <t>PUT</t>
-  </si>
-  <si>
-    <t>{root.api}/{version}/blog/post/:post-id</t>
-  </si>
-  <si>
-    <t>{
-    "kode":"200",
-    "message":"Successfully updated data",
-}</t>
-  </si>
-  <si>
-    <t>{
-    "kode":"400",
+    "code":"400",
     "message":"Body post tidak boleh memuat karakter khusus"
 }</t>
   </si>
@@ -216,13 +222,13 @@
   </si>
   <si>
     <t>{
-    "kode":"200",
-    "message":"Successfully deleted data",
+    "code":"200",
+    "message":"Successfully deleted data"
 }</t>
   </si>
   <si>
     <t>{
-    "kode":"400",
+    "code":"400",
     "message":"Id post tidak ditemukan"
 }</t>
   </si>
@@ -441,12 +447,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -767,7 +785,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -791,16 +809,16 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -809,89 +827,89 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -904,7 +922,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1442,16 +1475,16 @@
   <sheetPr/>
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="D5" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="6"/>
   <cols>
     <col min="1" max="2" width="14.1111111111111" customWidth="1"/>
     <col min="4" max="4" width="36" customWidth="1"/>
-    <col min="5" max="5" width="37.3333333333333" customWidth="1"/>
-    <col min="6" max="6" width="34.5555555555556" customWidth="1"/>
+    <col min="5" max="5" width="41.2222222222222" customWidth="1"/>
+    <col min="6" max="6" width="51.8888888888889" customWidth="1"/>
     <col min="7" max="7" width="36.6666666666667" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1496,145 +1529,148 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" ht="129.6" spans="1:7">
-      <c r="A4" s="3" t="s">
+    <row r="4" ht="115.2" spans="1:7">
+      <c r="A4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="6" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="5" ht="115.2" spans="1:7">
-      <c r="A5" s="3"/>
-      <c r="B5" t="s">
+      <c r="A5" s="4"/>
+      <c r="B5" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G5" s="6" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="6" ht="57.6" spans="1:7">
-      <c r="A6" s="3"/>
-      <c r="B6" t="s">
+      <c r="A6" s="4"/>
+      <c r="B6" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="G6" s="6" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="8" ht="115.2" spans="1:7">
-      <c r="A8" s="3" t="s">
+    <row r="8" ht="187.2" spans="1:7">
+      <c r="A8" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="G8" s="9" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="9" ht="72" spans="1:7">
-      <c r="A9" s="3"/>
-      <c r="B9" t="s">
+      <c r="A9" s="7"/>
+      <c r="B9" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="E9" s="8"/>
+      <c r="F9" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="G9" s="9" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="10" ht="72" spans="1:7">
-      <c r="A10" s="3"/>
-      <c r="B10" t="s">
+      <c r="A10" s="7"/>
+      <c r="B10" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="E10" s="8"/>
+      <c r="F10" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="G10" s="9" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="11" ht="57.6" spans="1:7">
-      <c r="A11" s="3"/>
-      <c r="B11" t="s">
+      <c r="A11" s="7"/>
+      <c r="B11" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="E11" s="8"/>
+      <c r="F11" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="G11" s="4" t="s">
+      <c r="G11" s="9" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1655,7 +1691,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="3"/>

</xml_diff>

<commit_message>
backend: MERN Project 31 - Menkoneksikan server MongoDB ke server Node JS
</commit_message>
<xml_diff>
--- a/backend/mern-api/docs/api-planning.xlsx
+++ b/backend/mern-api/docs/api-planning.xlsx
@@ -4,11 +4,13 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9000"/>
+    <workbookView windowWidth="23040" windowHeight="9000" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="API" sheetId="1" r:id="rId1"/>
     <sheet name="Response Status " sheetId="2" r:id="rId2"/>
+    <sheet name="Link" sheetId="3" r:id="rId3"/>
+    <sheet name="Database" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="66">
   <si>
     <t>Standar API</t>
   </si>
@@ -282,6 +284,21 @@
   </si>
   <si>
     <t>Invalid request from another request</t>
+  </si>
+  <si>
+    <t>Tutorial</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=nGWP07CtEx0&amp;list=PLU4DS8KR-LJ0-MT2QfV-fvJiNorsoFs74&amp;index=30</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=413C1PlYIko</t>
+  </si>
+  <si>
+    <t>ceepei14</t>
+  </si>
+  <si>
+    <t>hXvpMZrePqHSp2Yl</t>
   </si>
 </sst>
 </file>
@@ -1475,8 +1492,8 @@
   <sheetPr/>
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D5" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView topLeftCell="D5" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="6"/>
@@ -1807,4 +1824,61 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="2"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="1"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
backend: MERN Project 33 - Menyimpan Postingan Blog Ke Database MongoDB
</commit_message>
<xml_diff>
--- a/backend/mern-api/docs/api-planning.xlsx
+++ b/backend/mern-api/docs/api-planning.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9000" activeTab="3"/>
+    <workbookView windowWidth="23040" windowHeight="9000"/>
   </bookViews>
   <sheets>
     <sheet name="API" sheetId="1" r:id="rId1"/>
@@ -79,7 +79,7 @@
   </si>
   <si>
     <t>{
-    "code":"200",
+    "status":"200",
     "message":"Successfully registered access",
     "data":{
         "name":"Testing",
@@ -89,7 +89,7 @@
   </si>
   <si>
     <t>{
-    "code":"400",
+    "status":"400",
     "message":"email tidak valid"
 }</t>
   </si>
@@ -107,7 +107,7 @@
   </si>
   <si>
     <t>{
-    "code":"200",
+    "status":"200",
     "message":"Successfully login",
     "data":{
         "id":"123",
@@ -117,7 +117,7 @@
   </si>
   <si>
     <t>{
-    "code":"400",
+    "status":"400",
     "message":"Password salah"
 }</t>
   </si>
@@ -134,13 +134,13 @@
   </si>
   <si>
     <t>{
-    "code":"200",
+    "status":"200",
     "message":"Successfully logout"
 }</t>
   </si>
   <si>
     <t>{
-    "code":"500",
+    "status":"500",
     "message":"Internal Server Error"
 }</t>
   </si>
@@ -163,7 +163,7 @@
   </si>
   <si>
     <t>{
-    "code":"200",
+    "status":"200",
     "message":"Successfully added data",
     "data": {
             "title_post": "Harry potter book 1",  
@@ -178,7 +178,7 @@
   </si>
   <si>
     <t>{
-    "code":"400",
+    "status":"400",
     "message":"Judul post sudah ada"
 }</t>
   </si>
@@ -190,7 +190,7 @@
   </si>
   <si>
     <t>{
-    "code":"200",
+    "status":"200",
     "message":"Successfully updated data"
     "data": {}
 }</t>
@@ -206,13 +206,13 @@
   </si>
   <si>
     <t>{
-    "code":"200",
+    "status":"200",
     "message":"Successfully updated data"
 }</t>
   </si>
   <si>
     <t>{
-    "code":"400",
+    "status":"400",
     "message":"Body post tidak boleh memuat karakter khusus"
 }</t>
   </si>
@@ -224,13 +224,13 @@
   </si>
   <si>
     <t>{
-    "code":"200",
+    "status":"200",
     "message":"Successfully deleted data"
 }</t>
   </si>
   <si>
     <t>{
-    "code":"400",
+    "status":"400",
     "message":"Id post tidak ditemukan"
 }</t>
   </si>
@@ -1492,8 +1492,8 @@
   <sheetPr/>
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView topLeftCell="D5" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="D5" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="6"/>
@@ -1863,8 +1863,8 @@
   <sheetPr/>
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="1"/>

</xml_diff>

<commit_message>
frontend: MERN Project 45 - Integrasi penambahan post dan upload file
</commit_message>
<xml_diff>
--- a/backend/mern-api/docs/api-planning.xlsx
+++ b/backend/mern-api/docs/api-planning.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9000"/>
+    <workbookView windowWidth="23040" windowHeight="9000" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="API" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="67">
   <si>
     <t>Standar API</t>
   </si>
@@ -293,6 +293,9 @@
   </si>
   <si>
     <t>https://www.youtube.com/watch?v=413C1PlYIko</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/52427095/validating-file-presence-with-yup</t>
   </si>
   <si>
     <t>ceepei14</t>
@@ -1492,7 +1495,7 @@
   <sheetPr/>
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D5" workbookViewId="0">
+    <sheetView topLeftCell="D5" workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
@@ -1829,13 +1832,13 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="2"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="4"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
@@ -1850,6 +1853,11 @@
     <row r="3" spans="1:1">
       <c r="A3" t="s">
         <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -1871,10 +1879,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
backend: - Setup MySQL, membuat database baru dan table users - Membuat koneksi dari express ke MySQL Database - Refactor konfigurasi MySQL Connection
</commit_message>
<xml_diff>
--- a/backend/mern-api/docs/api-planning.xlsx
+++ b/backend/mern-api/docs/api-planning.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9000" activeTab="2"/>
+    <workbookView windowWidth="23040" windowHeight="9000"/>
   </bookViews>
   <sheets>
     <sheet name="API" sheetId="1" r:id="rId1"/>
@@ -1495,8 +1495,8 @@
   <sheetPr/>
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView topLeftCell="D5" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="D6" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="6"/>
@@ -1834,7 +1834,7 @@
   <sheetPr/>
   <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>

</xml_diff>